<commit_message>
Se actualiza archivo parametros comunicacion variador.xlsx
</commit_message>
<xml_diff>
--- a/Historial/parametros comunicacion variador.xlsx
+++ b/Historial/parametros comunicacion variador.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>B1-01</t>
   </si>
@@ -36,7 +36,19 @@
     <t>B1-02</t>
   </si>
   <si>
-    <t>El ejemplo que viene en el manual del variador esta incorrecto para el variador G5. El registro 0000h es la señal y 0001h es la frecuencia.</t>
+    <t>Reiniciar el variador al terminar de modificar los parametros para que los cambios tengan efecto.</t>
+  </si>
+  <si>
+    <t>Parametros de variador</t>
+  </si>
+  <si>
+    <t>Lavadora.net</t>
+  </si>
+  <si>
+    <t>El ejemplo que viene en el manual del variador esta incorrecto para el variador G5. El registro 0000h es la señal arranque/paro y 0001h es la frecuencia.</t>
+  </si>
+  <si>
+    <t>Mover selector de RS-422 a RS-485.</t>
   </si>
 </sst>
 </file>
@@ -60,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,86 +80,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -164,7 +136,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F4F4F4"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -443,69 +415,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="257" zoomScaleNormal="257" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="257" zoomScaleNormal="257" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
   </sheetData>
+  <sortState ref="B4:C9">
+    <sortCondition ref="B4:B9"/>
+  </sortState>
+  <mergeCells count="5">
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A13:D13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>